<commit_message>
Update on performance viz
</commit_message>
<xml_diff>
--- a/data/performance_sheets_option2/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets_option2/BA11 Overall Model Peformance Results.xlsx
@@ -770,19 +770,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.01083486617810965</v>
+        <v>0.0179918809253119</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.08131956240335234</v>
+        <v>0.1186304499816319</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.115278677226183</v>
+        <v>0.1696272826101057</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.1040906632609748</v>
+        <v>0.1341338172323143</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>12.28647850644498</v>
+        <v>18.00197642917625</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -800,19 +800,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.01114752394144978</v>
+        <v>0.03250270772802855</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.08270315887887283</v>
+        <v>0.1480394330773291</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1170547801815633</v>
+        <v>0.204227855967163</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1055818352816893</v>
+        <v>0.1802850735031288</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>12.25896537898139</v>
+        <v>23.89406442753663</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -2049,19 +2049,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>1.759931845161792</v>
+        <v>1.113949853911995</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>1.103913537280815</v>
+        <v>0.8811127075855789</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>780005209071857.9</v>
+        <v>1239582830352277</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.326624229072344</v>
+        <v>1.055438228373407</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>124.8448018444424</v>
+        <v>130.7315789378721</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -2079,19 +2079,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>2.791898086873211</v>
+        <v>1.970900756794443</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>1.331759497535043</v>
+        <v>1.1365416461419</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>886326517985504.9</v>
+        <v>1878223606308148</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>1.670897389690106</v>
+        <v>1.403887729412307</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>129.6261458255306</v>
+        <v>127.2944179994935</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -3325,19 +3325,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>2.753413270073988</v>
+        <v>2.626297509864584</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>1.446948021752789</v>
+        <v>1.307411706232485</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>921528962281436.9</v>
+        <v>1924762208522051</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.659341215685908</v>
+        <v>1.620585545370742</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>140.1184587649541</v>
+        <v>147.5295062912983</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -3355,19 +3355,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>2.776867631597437</v>
+        <v>8.961966498157992</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>1.46963174230184</v>
+        <v>2.399776615514196</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>989071866954009.6</v>
+        <v>3207652147597913</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>1.666393600443016</v>
+        <v>2.99365437186025</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>140.4866553360677</v>
+        <v>164.287008092179</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -4601,19 +4601,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>1.078076408077252</v>
+        <v>2.187003232381139</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.7996622523418322</v>
+        <v>1.260030062154847</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.7996622523418322</v>
+        <v>1372020673264916</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.038304583480807</v>
+        <v>1.47885199813272</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>98.67612280092682</v>
+        <v>192.6092387796874</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -4631,19 +4631,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>1.418180110641853</v>
+        <v>3.749116858523515</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>1.005428551320527</v>
+        <v>1.618175000014997</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>1.005428551320527</v>
+        <v>2895850310827128</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>1.190873675350099</v>
+        <v>1.936263633528119</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>132.2777904092138</v>
+        <v>182.2623187051494</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -5875,19 +5875,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0430522201908769</v>
+        <v>0.04905374744615793</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1314835993100613</v>
+        <v>0.1348942525282142</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.959904367424433</v>
+        <v>1.180031753678706</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2074902893893518</v>
+        <v>0.2214808060445824</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>27.11927964937372</v>
+        <v>27.47842772577463</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -5905,19 +5905,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.0424112916118266</v>
+        <v>0.04854120948959907</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1324733819963559</v>
+        <v>0.1344970376261711</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.946806843529418</v>
+        <v>1.17341376202927</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2059400194518458</v>
+        <v>0.220320696916107</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>27.29303617570489</v>
+        <v>27.49387665851739</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -7149,19 +7149,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0311340201761948</v>
+        <v>0.03076230876773942</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1239726508952864</v>
+        <v>0.10065807139648</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.5912703663693335</v>
+        <v>1.061274415764125</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.1764483498823234</v>
+        <v>0.1753918720116169</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>25.62839514847395</v>
+        <v>22.56021813802044</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -7179,19 +7179,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.0271620764928708</v>
+        <v>0.03082799117911534</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1122267573154565</v>
+        <v>0.1006783586476175</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.54409260263257</v>
+        <v>1.063519356121315</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1648092124029201</v>
+        <v>0.1755790169100948</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>23.76928835945012</v>
+        <v>22.56724825816929</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -8423,19 +8423,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0261124182783155</v>
+        <v>0.03145118012700405</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1173685595042552</v>
+        <v>0.1176109511430981</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.3756395666746478</v>
+        <v>1.064104257804336</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.1615933732500052</v>
+        <v>0.1773448057514063</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>23.1989021675348</v>
+        <v>28.0377848840399</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -8453,19 +8453,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.0354158088235058</v>
+        <v>0.02877552441652384</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1487976966598559</v>
+        <v>0.1025793405321778</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.4955116733198275</v>
+        <v>1.05677053477698</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1881908840074509</v>
+        <v>0.169633500277875</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>29.22681436703406</v>
+        <v>23.62401367184036</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -9697,19 +9697,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.4203045185773763</v>
+        <v>0.5211246120532131</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.3015176564988622</v>
+        <v>0.3336833755184812</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.5401393397574145</v>
+        <v>0.5727384682036503</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.6483089684536042</v>
+        <v>0.7218896120967617</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>15.15559508346164</v>
+        <v>16.81272907165241</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -9727,19 +9727,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.4203267594318844</v>
+        <v>0.5209976961238756</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.3015265789629142</v>
+        <v>0.3336778446090488</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.5401578127346061</v>
+        <v>0.5726927452202003</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.6483261212012704</v>
+        <v>0.7218017013861048</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>15.15588837815034</v>
+        <v>16.8131097436111</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -10971,19 +10971,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.2199517292721804</v>
+        <v>0.3963140912831225</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2595831934151383</v>
+        <v>0.269534297037626</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.4555008349380663</v>
+        <v>0.5259475840008978</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.4689901163907192</v>
+        <v>0.629534821342809</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>13.25567789401703</v>
+        <v>14.41449720095513</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -11001,19 +11001,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.262038833152892</v>
+        <v>0.4397589409703375</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2900195378344591</v>
+        <v>0.2802417544319984</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.4957012065002503</v>
+        <v>0.551743323697844</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.5118972876983156</v>
+        <v>0.6631432280965684</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>14.50774462231684</v>
+        <v>14.86114731823628</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -12245,19 +12245,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.1960912724530271</v>
+        <v>0.3341419342718551</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.3184881205582272</v>
+        <v>0.2808505500743309</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.432644090589835</v>
+        <v>0.2446381002270317</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.4428219421539848</v>
+        <v>0.5780501139796229</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>15.69572929145428</v>
+        <v>14.38313770986017</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -12275,19 +12275,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.1931980752359565</v>
+        <v>0.340126881879963</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.3001605587319769</v>
+        <v>0.290135949221715</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.4527120094199768</v>
+        <v>0.2495320181462332</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.4395430300163529</v>
+        <v>0.5832039796503132</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>14.80395344519196</v>
+        <v>14.79341989135393</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -13519,19 +13519,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0645296532555998</v>
+        <v>0.04024338070258342</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1838226737594122</v>
+        <v>0.1568905693894855</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.2820745923573743</v>
+        <v>0.2316665929312102</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2540268750656115</v>
+        <v>0.2006075290276599</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>24.2144846008716</v>
+        <v>21.58477685365705</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -14523,19 +14523,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.01969885289882036</v>
+        <v>0.0281175482060782</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1174275115376849</v>
+        <v>0.1279678585492715</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.3360830868041156</v>
+        <v>0.1902326352532762</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.14035260203794</v>
+        <v>0.1676828798836608</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>22.33034058473802</v>
+        <v>20.21080586637246</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -14553,19 +14553,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.02100868539704847</v>
+        <v>0.02466042671762571</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1190628989812463</v>
+        <v>0.1113212340714586</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.3443383137597342</v>
+        <v>0.171858315769591</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1449437318308331</v>
+        <v>0.1570363866039515</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>22.39794543747536</v>
+        <v>17.67252413352941</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -15797,19 +15797,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.1151604168057459</v>
+        <v>0.1713580497920794</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2638231695688058</v>
+        <v>0.3414249082301279</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.468824896705242</v>
+        <v>0.5415784986528271</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.3393529384074137</v>
+        <v>0.4139541638781755</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>38.42080202741158</v>
+        <v>68.92945276192613</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -16801,19 +16801,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>4.62621638182031</v>
+        <v>2.015034735724734</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>1.744527234925574</v>
+        <v>1.017926757261285</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>3.394696005874605</v>
+        <v>2.42821152037283</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>2.150864101197542</v>
+        <v>1.419519191742307</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>127.1517229351176</v>
+        <v>114.935707975681</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -17805,19 +17805,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.5990497117314423</v>
+        <v>0.9417912160220516</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.6456588223021085</v>
+        <v>0.7595408877367373</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.2360510137038637</v>
+        <v>0.2704198110401613</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.7739830177280651</v>
+        <v>0.97045928097064</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>23.45293629766138</v>
+        <v>25.44736189641421</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -18809,19 +18809,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>1.445541661146428</v>
+        <v>4.748770044021249</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.9699710096383446</v>
+        <v>1.75983036844142</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.3895383410771646</v>
+        <v>0.6583525225842659</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.202306808242567</v>
+        <v>2.179167282248256</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>49.31778542496008</v>
+        <v>84.51012561520299</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -19813,19 +19813,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>1.141950600337144</v>
+        <v>1.145750813661144</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.8728222787630854</v>
+        <v>0.8071426284398897</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.371189287193554</v>
+        <v>0.3005445726125022</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.068620887095674</v>
+        <v>1.070397502641492</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>34.67208524643041</v>
+        <v>33.14846474252346</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -20817,19 +20817,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.01406539273791445</v>
+        <v>0.01287121123128601</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.09906829029398519</v>
+        <v>0.08563202834452491</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.1946154420798608</v>
+        <v>0.1181390320346846</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.1185976084831159</v>
+        <v>0.1134513606409637</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>18.38679593006343</v>
+        <v>12.53255944509988</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -20847,19 +20847,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.01391261674581112</v>
+        <v>0.01998722168110157</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.09487512448385897</v>
+        <v>0.1209672007108275</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1868784524602167</v>
+        <v>0.1790174201338875</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1179517560098667</v>
+        <v>0.1413761708390122</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>18.17035625504726</v>
+        <v>19.98701887951244</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -22091,19 +22091,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.048316468459003</v>
+        <v>0.08879198112204009</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1694676104225125</v>
+        <v>0.2651541837938986</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.06213894336527613</v>
+        <v>0.09584498273079374</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2198100736067458</v>
+        <v>0.297979833415015</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>6.545036720881969</v>
+        <v>9.926561799027152</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -22121,19 +22121,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.06532770124223965</v>
+        <v>0.1329966971440318</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2176379471667126</v>
+        <v>0.2993721930238203</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.0800181718831763</v>
+        <v>0.1081281580231559</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.255592842705424</v>
+        <v>0.3646871222624015</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>8.342026550686112</v>
+        <v>11.74463826906958</v>
       </c>
     </row>
     <row r="8" ht="28.5" customHeight="1">
@@ -23366,19 +23366,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.1082531958982518</v>
+        <v>0.1049348382747722</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1965125657240989</v>
+        <v>0.2151390074506735</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.1203141121301667</v>
+        <v>0.09334073671045441</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.3290185342777087</v>
+        <v>0.323936472591112</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>9.043985868342967</v>
+        <v>8.909510778174404</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -23396,19 +23396,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.103278569665368</v>
+        <v>0.1319980439940538</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.186497082411782</v>
+        <v>0.2680672671904306</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1147691552271435</v>
+        <v>0.1062093585897546</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.3213698331601272</v>
+        <v>0.3633153506171379</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>8.569319475200201</v>
+        <v>10.71208133155415</v>
       </c>
     </row>
     <row r="8" ht="28.5" customHeight="1">
@@ -24641,19 +24641,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.07847006953330807</v>
+        <v>0.07472352836974828</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2208546989376738</v>
+        <v>0.1919161812161036</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.09212300467943695</v>
+        <v>0.06744969770511261</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2801250962218631</v>
+        <v>0.2733560468871107</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>8.827458750749523</v>
+        <v>7.178312920982592</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -24671,19 +24671,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.07871205045427121</v>
+        <v>0.1029953252738324</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2302559149929638</v>
+        <v>0.2359410632715214</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.09460522492317136</v>
+        <v>0.08245310106045689</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2805566795752174</v>
+        <v>0.3209288476809656</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>8.98570547227677</v>
+        <v>8.874698031978594</v>
       </c>
     </row>
     <row r="8" ht="28.5" customHeight="1">
@@ -25918,19 +25918,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.3089474454304963</v>
+        <v>1.056994605137028</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.4413260507627003</v>
+        <v>0.858724435680976</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.4413260507627003</v>
+        <v>883717275121979.8</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.5558304106744217</v>
+        <v>1.028102429302172</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>68.15596179692702</v>
+        <v>177.0027571523113</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -25948,19 +25948,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.3116463054447938</v>
+        <v>1.033145897545401</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.492336968327487</v>
+        <v>0.8566940721454438</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.492336968327487</v>
+        <v>831400841312325.9</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.5582529045556268</v>
+        <v>1.016437847359789</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>74.04756743125425</v>
+        <v>180.5183506677184</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -27196,19 +27196,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.3310183876323539</v>
+        <v>0.4051472972625934</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.4272663328668611</v>
+        <v>0.4894173230022899</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>634959794087088.5</v>
+        <v>1072036993429984</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.5753419745093815</v>
+        <v>0.6365118202065013</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>64.16331125097351</v>
+        <v>83.26798026807425</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -27226,19 +27226,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.3344083303762097</v>
+        <v>0.4176178695573639</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.459242139059459</v>
+        <v>0.5207142485266109</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>553487132637237.9</v>
+        <v>1196903332573756</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.5782804945493231</v>
+        <v>0.6462336029311412</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>68.37322933735668</v>
+        <v>81.66427961802161</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -28472,19 +28472,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.6909267407057833</v>
+        <v>1.016765273733438</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.6721864021675006</v>
+        <v>0.8550418001520068</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>553660153051136.7</v>
+        <v>870896314341999</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.8312200314632602</v>
+        <v>1.008347794034101</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>91.93624763359816</v>
+        <v>159.8109631189442</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -28502,19 +28502,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.9833028862534986</v>
+        <v>1.203211406246794</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.7789156211042709</v>
+        <v>0.9222647529419414</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>549984794219508.6</v>
+        <v>826020043883285</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.9916162999131763</v>
+        <v>1.096909935339631</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>95.27313080289623</v>
+        <v>167.2729577605253</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">

</xml_diff>